<commit_message>
Update sprint artifact description
</commit_message>
<xml_diff>
--- a/docs/Requirements.xlsx
+++ b/docs/Requirements.xlsx
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="186">
   <si>
     <t>Reference Story No</t>
   </si>
@@ -551,7 +551,7 @@
     <t>1.5 hrs</t>
   </si>
   <si>
-    <t>Create State Diagram UML Diagram</t>
+    <t>Create a UML state diagram that describes how the state of the website changes based on various user inputs.</t>
   </si>
   <si>
     <t>Summarize front-end, back-end, and data flow of the application. Include technologies used, crucial connections between front-end and back-end, and give reader a comprehensive  view of how program works.</t>
@@ -3119,7 +3119,7 @@
         <v>45.0</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>166</v>
+        <v>100</v>
       </c>
       <c r="C16" s="7">
         <v>5.0</v>
@@ -3130,7 +3130,9 @@
       <c r="E16" s="7">
         <v>1.0</v>
       </c>
-      <c r="F16" s="28"/>
+      <c r="F16" s="17" t="s">
+        <v>166</v>
+      </c>
       <c r="G16" s="7" t="s">
         <v>88</v>
       </c>

</xml_diff>